<commit_message>
Update Variables to include in global and site reports_Curacao_20250327.xlsx
Removed dc, pd continuous age in days
</commit_message>
<xml_diff>
--- a/Variables to include in global and site reports_Curacao_20250327.xlsx
+++ b/Variables to include in global and site reports_Curacao_20250327.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dave_\Box\Projects\RMHC on Box\RMHC_Curacao_data_to_global\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49350923-D515-4AC8-AF3C-A6EC3860FC35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC2550F-D4D7-4E53-90AB-471A62D89C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37185" yWindow="585" windowWidth="20190" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40725" yWindow="2505" windowWidth="15405" windowHeight="14775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Use this tab" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3111" uniqueCount="1320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3105" uniqueCount="1320">
   <si>
     <t>Variable Name</t>
   </si>
@@ -4511,10 +4511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E817332-1EA0-456A-B825-F5C8D62F83CA}">
-  <dimension ref="A1:E321"/>
+  <dimension ref="A1:E319"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:E8"/>
+    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
+      <selection activeCell="A236" sqref="A236:XFD236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6577,44 +6577,42 @@
       </c>
       <c r="E178" s="23"/>
     </row>
-    <row r="179" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A179" s="23" t="s">
-        <v>275</v>
-      </c>
-      <c r="B179" s="23" t="s">
-        <v>276</v>
-      </c>
-      <c r="C179" s="23"/>
+    <row r="179" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A179" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="B179" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="C179" s="23" t="s">
+        <v>46</v>
+      </c>
       <c r="D179" s="23"/>
-      <c r="E179" s="23" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A180" s="22" t="s">
-        <v>278</v>
-      </c>
-      <c r="B180" s="22" t="s">
-        <v>278</v>
+      <c r="E179" s="23"/>
+    </row>
+    <row r="180" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A180" s="23" t="s">
+        <v>279</v>
+      </c>
+      <c r="B180" s="23" t="s">
+        <v>81</v>
       </c>
       <c r="C180" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="D180" s="23"/>
+        <v>82</v>
+      </c>
+      <c r="D180" s="23" t="s">
+        <v>83</v>
+      </c>
       <c r="E180" s="23"/>
     </row>
-    <row r="181" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" s="23" t="s">
         <v>279</v>
       </c>
-      <c r="B181" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="C181" s="23" t="s">
-        <v>82</v>
-      </c>
+      <c r="B181" s="23"/>
+      <c r="C181" s="23"/>
       <c r="D181" s="23" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E181" s="23"/>
     </row>
@@ -6625,7 +6623,7 @@
       <c r="B182" s="23"/>
       <c r="C182" s="23"/>
       <c r="D182" s="23" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E182" s="23"/>
     </row>
@@ -6636,7 +6634,7 @@
       <c r="B183" s="23"/>
       <c r="C183" s="23"/>
       <c r="D183" s="23" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E183" s="23"/>
     </row>
@@ -6647,100 +6645,100 @@
       <c r="B184" s="23"/>
       <c r="C184" s="23"/>
       <c r="D184" s="23" t="s">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="E184" s="23"/>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A185" s="23" t="s">
-        <v>279</v>
+      <c r="A185" s="22" t="s">
+        <v>280</v>
       </c>
       <c r="B185" s="23"/>
       <c r="C185" s="23"/>
-      <c r="D185" s="23" t="s">
-        <v>44</v>
-      </c>
+      <c r="D185" s="23"/>
       <c r="E185" s="23"/>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A186" s="22" t="s">
-        <v>280</v>
-      </c>
-      <c r="B186" s="23"/>
-      <c r="C186" s="23"/>
+    <row r="186" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A186" s="23" t="s">
+        <v>281</v>
+      </c>
+      <c r="B186" s="23" t="s">
+        <v>282</v>
+      </c>
+      <c r="C186" s="23" t="s">
+        <v>126</v>
+      </c>
       <c r="D186" s="23"/>
       <c r="E186" s="23"/>
     </row>
-    <row r="187" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A187" s="23" t="s">
-        <v>281</v>
-      </c>
-      <c r="B187" s="23" t="s">
-        <v>282</v>
-      </c>
+    <row r="187" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A187" s="22" t="s">
+        <v>283</v>
+      </c>
+      <c r="B187" s="23"/>
       <c r="C187" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="D187" s="23"/>
+        <v>145</v>
+      </c>
+      <c r="D187" s="23" t="s">
+        <v>146</v>
+      </c>
       <c r="E187" s="23"/>
     </row>
-    <row r="188" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A188" s="22" t="s">
-        <v>283</v>
-      </c>
-      <c r="B188" s="23"/>
+    <row r="188" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A188" s="23" t="s">
+        <v>284</v>
+      </c>
+      <c r="B188" s="23" t="s">
+        <v>148</v>
+      </c>
       <c r="C188" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="D188" s="23" t="s">
-        <v>146</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="D188" s="23"/>
       <c r="E188" s="23"/>
     </row>
     <row r="189" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A189" s="23" t="s">
         <v>284</v>
       </c>
-      <c r="B189" s="23" t="s">
-        <v>148</v>
-      </c>
+      <c r="B189" s="23"/>
       <c r="C189" s="23" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D189" s="23"/>
       <c r="E189" s="23"/>
     </row>
-    <row r="190" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A190" s="23" t="s">
         <v>284</v>
       </c>
       <c r="B190" s="23"/>
       <c r="C190" s="23" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D190" s="23"/>
       <c r="E190" s="23"/>
     </row>
     <row r="191" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A191" s="23" t="s">
-        <v>284</v>
-      </c>
-      <c r="B191" s="23"/>
+        <v>285</v>
+      </c>
+      <c r="B191" s="23" t="s">
+        <v>155</v>
+      </c>
       <c r="C191" s="23" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D191" s="23"/>
       <c r="E191" s="23"/>
     </row>
     <row r="192" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A192" s="23" t="s">
-        <v>285</v>
-      </c>
-      <c r="B192" s="23" t="s">
-        <v>155</v>
-      </c>
+        <v>286</v>
+      </c>
+      <c r="B192" s="23"/>
       <c r="C192" s="23" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="D192" s="23"/>
       <c r="E192" s="23"/>
@@ -6751,7 +6749,7 @@
       </c>
       <c r="B193" s="23"/>
       <c r="C193" s="23" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D193" s="23"/>
       <c r="E193" s="23"/>
@@ -6762,7 +6760,7 @@
       </c>
       <c r="B194" s="23"/>
       <c r="C194" s="23" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D194" s="23"/>
       <c r="E194" s="23"/>
@@ -6773,51 +6771,49 @@
       </c>
       <c r="B195" s="23"/>
       <c r="C195" s="23" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D195" s="23"/>
       <c r="E195" s="23"/>
     </row>
-    <row r="196" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A196" s="23" t="s">
-        <v>286</v>
-      </c>
-      <c r="B196" s="23"/>
+        <v>287</v>
+      </c>
+      <c r="B196" s="23" t="s">
+        <v>288</v>
+      </c>
       <c r="C196" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="D196" s="23"/>
+        <v>161</v>
+      </c>
+      <c r="D196" s="23" t="s">
+        <v>116</v>
+      </c>
       <c r="E196" s="23"/>
     </row>
-    <row r="197" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" s="23" t="s">
         <v>287</v>
       </c>
-      <c r="B197" s="23" t="s">
-        <v>288</v>
-      </c>
-      <c r="C197" s="23" t="s">
-        <v>161</v>
-      </c>
+      <c r="B197" s="23"/>
+      <c r="C197" s="23"/>
       <c r="D197" s="23" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E197" s="23"/>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A198" s="23" t="s">
-        <v>287</v>
+      <c r="A198" s="22" t="s">
+        <v>289</v>
       </c>
       <c r="B198" s="23"/>
       <c r="C198" s="23"/>
-      <c r="D198" s="23" t="s">
-        <v>117</v>
-      </c>
+      <c r="D198" s="23"/>
       <c r="E198" s="23"/>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" s="22" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B199" s="23"/>
       <c r="C199" s="23"/>
@@ -6826,7 +6822,7 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200" s="22" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B200" s="23"/>
       <c r="C200" s="23"/>
@@ -6835,7 +6831,7 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201" s="22" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B201" s="23"/>
       <c r="C201" s="23"/>
@@ -6844,65 +6840,65 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A202" s="22" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B202" s="23"/>
       <c r="C202" s="23"/>
       <c r="D202" s="23"/>
       <c r="E202" s="23"/>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A203" s="22" t="s">
-        <v>293</v>
-      </c>
-      <c r="B203" s="23"/>
+    <row r="203" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A203" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="B203" s="23" t="s">
+        <v>168</v>
+      </c>
       <c r="C203" s="23"/>
       <c r="D203" s="23"/>
       <c r="E203" s="23"/>
     </row>
-    <row r="204" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A204" s="23" t="s">
-        <v>294</v>
-      </c>
-      <c r="B204" s="23" t="s">
-        <v>168</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="B204" s="23"/>
       <c r="C204" s="23"/>
       <c r="D204" s="23"/>
       <c r="E204" s="23"/>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A205" s="23" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B205" s="23"/>
       <c r="C205" s="23"/>
       <c r="D205" s="23"/>
       <c r="E205" s="23"/>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A206" s="23" t="s">
-        <v>296</v>
-      </c>
-      <c r="B206" s="23"/>
+        <v>297</v>
+      </c>
+      <c r="B206" s="23" t="s">
+        <v>185</v>
+      </c>
       <c r="C206" s="23"/>
       <c r="D206" s="23"/>
       <c r="E206" s="23"/>
     </row>
-    <row r="207" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A207" s="23" t="s">
-        <v>297</v>
-      </c>
-      <c r="B207" s="23" t="s">
-        <v>185</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="B207" s="23"/>
       <c r="C207" s="23"/>
       <c r="D207" s="23"/>
       <c r="E207" s="23"/>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A208" s="23" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B208" s="23"/>
       <c r="C208" s="23"/>
@@ -6911,7 +6907,7 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" s="23" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B209" s="23"/>
       <c r="C209" s="23"/>
@@ -6920,7 +6916,7 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" s="23" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B210" s="23"/>
       <c r="C210" s="23"/>
@@ -6929,7 +6925,7 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" s="23" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B211" s="23"/>
       <c r="C211" s="23"/>
@@ -6938,7 +6934,7 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" s="23" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B212" s="23"/>
       <c r="C212" s="23"/>
@@ -6947,7 +6943,7 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" s="23" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B213" s="23"/>
       <c r="C213" s="23"/>
@@ -6956,7 +6952,7 @@
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" s="23" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B214" s="23"/>
       <c r="C214" s="23"/>
@@ -6965,45 +6961,49 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" s="23" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B215" s="23"/>
       <c r="C215" s="23"/>
       <c r="D215" s="23"/>
       <c r="E215" s="23"/>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A216" s="23" t="s">
-        <v>306</v>
-      </c>
-      <c r="B216" s="23"/>
+        <v>307</v>
+      </c>
+      <c r="B216" s="23" t="s">
+        <v>308</v>
+      </c>
       <c r="C216" s="23"/>
-      <c r="D216" s="23"/>
-      <c r="E216" s="23"/>
-    </row>
-    <row r="217" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="D216" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E216" s="23" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" s="23" t="s">
         <v>307</v>
       </c>
-      <c r="B217" s="23" t="s">
-        <v>308</v>
-      </c>
+      <c r="B217" s="23"/>
       <c r="C217" s="23"/>
       <c r="D217" s="23" t="s">
-        <v>207</v>
-      </c>
-      <c r="E217" s="23" t="s">
-        <v>309</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="E217" s="23"/>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218" s="23" t="s">
-        <v>307</v>
-      </c>
-      <c r="B218" s="23"/>
+        <v>310</v>
+      </c>
+      <c r="B218" s="23" t="s">
+        <v>311</v>
+      </c>
       <c r="C218" s="23"/>
       <c r="D218" s="23" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E218" s="23"/>
     </row>
@@ -7011,47 +7011,47 @@
       <c r="A219" s="23" t="s">
         <v>310</v>
       </c>
-      <c r="B219" s="23" t="s">
-        <v>311</v>
-      </c>
+      <c r="B219" s="23"/>
       <c r="C219" s="23"/>
       <c r="D219" s="23" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E219" s="23"/>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A220" s="23" t="s">
-        <v>310</v>
-      </c>
-      <c r="B220" s="23"/>
+        <v>312</v>
+      </c>
+      <c r="B220" s="23" t="s">
+        <v>213</v>
+      </c>
       <c r="C220" s="23"/>
       <c r="D220" s="23" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E220" s="23"/>
     </row>
-    <row r="221" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221" s="23" t="s">
         <v>312</v>
       </c>
-      <c r="B221" s="23" t="s">
-        <v>213</v>
-      </c>
+      <c r="B221" s="23"/>
       <c r="C221" s="23"/>
       <c r="D221" s="23" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E221" s="23"/>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" s="23" t="s">
-        <v>312</v>
-      </c>
-      <c r="B222" s="23"/>
+        <v>313</v>
+      </c>
+      <c r="B222" s="23" t="s">
+        <v>44</v>
+      </c>
       <c r="C222" s="23"/>
       <c r="D222" s="23" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E222" s="23"/>
     </row>
@@ -7059,74 +7059,72 @@
       <c r="A223" s="23" t="s">
         <v>313</v>
       </c>
-      <c r="B223" s="23" t="s">
-        <v>44</v>
-      </c>
+      <c r="B223" s="23"/>
       <c r="C223" s="23"/>
       <c r="D223" s="23" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E223" s="23"/>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A224" s="23" t="s">
-        <v>313</v>
+      <c r="A224" s="22" t="s">
+        <v>314</v>
       </c>
       <c r="B224" s="23"/>
       <c r="C224" s="23"/>
-      <c r="D224" s="23" t="s">
-        <v>209</v>
-      </c>
+      <c r="D224" s="23"/>
       <c r="E224" s="23"/>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A225" s="22" t="s">
-        <v>314</v>
-      </c>
-      <c r="B225" s="23"/>
+    <row r="225" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A225" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="B225" s="23" t="s">
+        <v>251</v>
+      </c>
       <c r="C225" s="23"/>
       <c r="D225" s="23"/>
       <c r="E225" s="23"/>
     </row>
     <row r="226" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A226" s="23" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B226" s="23" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C226" s="23"/>
       <c r="D226" s="23"/>
       <c r="E226" s="23"/>
     </row>
-    <row r="227" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A227" s="23" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B227" s="23" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C227" s="23"/>
       <c r="D227" s="23"/>
       <c r="E227" s="23"/>
     </row>
-    <row r="228" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A228" s="23" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B228" s="23" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C228" s="23"/>
       <c r="D228" s="23"/>
       <c r="E228" s="23"/>
     </row>
-    <row r="229" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A229" s="23" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B229" s="23" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C229" s="23"/>
       <c r="D229" s="23"/>
@@ -7134,10 +7132,10 @@
     </row>
     <row r="230" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A230" s="23" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B230" s="23" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C230" s="23"/>
       <c r="D230" s="23"/>
@@ -7145,198 +7143,196 @@
     </row>
     <row r="231" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A231" s="23" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B231" s="23" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C231" s="23"/>
       <c r="D231" s="23"/>
       <c r="E231" s="23"/>
     </row>
-    <row r="232" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A232" s="23" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B232" s="23" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C232" s="23"/>
       <c r="D232" s="23"/>
       <c r="E232" s="23"/>
     </row>
-    <row r="233" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A233" s="23" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B233" s="23" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C233" s="23"/>
       <c r="D233" s="23"/>
       <c r="E233" s="23"/>
     </row>
-    <row r="234" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A234" s="23" t="s">
-        <v>323</v>
-      </c>
-      <c r="B234" s="23" t="s">
-        <v>267</v>
-      </c>
+        <v>324</v>
+      </c>
+      <c r="B234" s="23"/>
       <c r="C234" s="23"/>
       <c r="D234" s="23"/>
       <c r="E234" s="23"/>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A235" s="23" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B235" s="23"/>
       <c r="C235" s="23"/>
       <c r="D235" s="23"/>
       <c r="E235" s="23"/>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A236" s="23" t="s">
-        <v>325</v>
-      </c>
-      <c r="B236" s="23"/>
+        <v>328</v>
+      </c>
+      <c r="B236" s="23" t="s">
+        <v>329</v>
+      </c>
       <c r="C236" s="23"/>
-      <c r="D236" s="23"/>
+      <c r="D236" s="23" t="s">
+        <v>330</v>
+      </c>
       <c r="E236" s="23"/>
     </row>
-    <row r="237" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A237" s="23" t="s">
-        <v>326</v>
-      </c>
-      <c r="B237" s="23" t="s">
-        <v>327</v>
-      </c>
+        <v>328</v>
+      </c>
+      <c r="B237" s="23"/>
       <c r="C237" s="23"/>
-      <c r="D237" s="23"/>
-      <c r="E237" s="23" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="238" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="D237" s="23" t="s">
+        <v>331</v>
+      </c>
+      <c r="E237" s="23"/>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A238" s="23" t="s">
         <v>328</v>
       </c>
-      <c r="B238" s="23" t="s">
-        <v>329</v>
-      </c>
+      <c r="B238" s="23"/>
       <c r="C238" s="23"/>
       <c r="D238" s="23" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="E238" s="23"/>
     </row>
-    <row r="239" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A239" s="23" t="s">
         <v>328</v>
       </c>
       <c r="B239" s="23"/>
       <c r="C239" s="23"/>
       <c r="D239" s="23" t="s">
-        <v>331</v>
+        <v>44</v>
       </c>
       <c r="E239" s="23"/>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A240" s="23" t="s">
-        <v>328</v>
-      </c>
-      <c r="B240" s="23"/>
+        <v>333</v>
+      </c>
+      <c r="B240" s="23" t="s">
+        <v>334</v>
+      </c>
       <c r="C240" s="23"/>
       <c r="D240" s="23" t="s">
-        <v>332</v>
+        <v>116</v>
       </c>
       <c r="E240" s="23"/>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A241" s="23" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="B241" s="23"/>
       <c r="C241" s="23"/>
       <c r="D241" s="23" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="E241" s="23"/>
     </row>
     <row r="242" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A242" s="23" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B242" s="23" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C242" s="23"/>
-      <c r="D242" s="23" t="s">
+      <c r="D242" s="23"/>
+      <c r="E242" s="23"/>
+    </row>
+    <row r="243" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A243" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="B243" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="C243" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="E242" s="23"/>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A243" s="23" t="s">
-        <v>333</v>
-      </c>
-      <c r="B243" s="23"/>
-      <c r="C243" s="23"/>
-      <c r="D243" s="23" t="s">
+      <c r="D243" s="23"/>
+      <c r="E243" s="23"/>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A244" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="B244" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="C244" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="E243" s="23"/>
-    </row>
-    <row r="244" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A244" s="23" t="s">
-        <v>335</v>
-      </c>
-      <c r="B244" s="23" t="s">
-        <v>336</v>
-      </c>
-      <c r="C244" s="23"/>
       <c r="D244" s="23"/>
       <c r="E244" s="23"/>
     </row>
     <row r="245" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A245" s="23" t="s">
-        <v>272</v>
+        <v>337</v>
       </c>
       <c r="B245" s="23" t="s">
-        <v>273</v>
+        <v>81</v>
       </c>
       <c r="C245" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="D245" s="23"/>
+        <v>82</v>
+      </c>
+      <c r="D245" s="23" t="s">
+        <v>83</v>
+      </c>
       <c r="E245" s="23"/>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A246" s="23" t="s">
-        <v>272</v>
-      </c>
-      <c r="B246" s="23" t="s">
-        <v>272</v>
-      </c>
-      <c r="C246" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="D246" s="23"/>
+        <v>337</v>
+      </c>
+      <c r="B246" s="23"/>
+      <c r="C246" s="23"/>
+      <c r="D246" s="23" t="s">
+        <v>84</v>
+      </c>
       <c r="E246" s="23"/>
     </row>
-    <row r="247" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A247" s="23" t="s">
         <v>337</v>
       </c>
-      <c r="B247" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="C247" s="23" t="s">
-        <v>82</v>
-      </c>
+      <c r="B247" s="23"/>
+      <c r="C247" s="23"/>
       <c r="D247" s="23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E247" s="23"/>
     </row>
@@ -7347,7 +7343,7 @@
       <c r="B248" s="23"/>
       <c r="C248" s="23"/>
       <c r="D248" s="23" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E248" s="23"/>
     </row>
@@ -7358,162 +7354,158 @@
       <c r="B249" s="23"/>
       <c r="C249" s="23"/>
       <c r="D249" s="23" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
       <c r="E249" s="23"/>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A250" s="23" t="s">
-        <v>337</v>
-      </c>
-      <c r="B250" s="23"/>
-      <c r="C250" s="23"/>
+        <v>338</v>
+      </c>
+      <c r="B250" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C250" s="23" t="s">
+        <v>89</v>
+      </c>
       <c r="D250" s="23" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E250" s="23"/>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A251" s="23" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B251" s="23"/>
       <c r="C251" s="23"/>
       <c r="D251" s="23" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="E251" s="23"/>
     </row>
-    <row r="252" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A252" s="23" t="s">
-        <v>338</v>
-      </c>
-      <c r="B252" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="C252" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="D252" s="23" t="s">
-        <v>90</v>
-      </c>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A252" s="22" t="s">
+        <v>339</v>
+      </c>
+      <c r="B252" s="23"/>
+      <c r="C252" s="23"/>
+      <c r="D252" s="23"/>
       <c r="E252" s="23"/>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A253" s="23" t="s">
-        <v>338</v>
-      </c>
-      <c r="B253" s="23"/>
+        <v>340</v>
+      </c>
+      <c r="B253" s="23" t="s">
+        <v>341</v>
+      </c>
       <c r="C253" s="23"/>
-      <c r="D253" s="23" t="s">
-        <v>91</v>
-      </c>
+      <c r="D253" s="23"/>
       <c r="E253" s="23"/>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A254" s="22" t="s">
-        <v>339</v>
-      </c>
-      <c r="B254" s="23"/>
+        <v>342</v>
+      </c>
+      <c r="B254" s="23" t="s">
+        <v>343</v>
+      </c>
       <c r="C254" s="23"/>
       <c r="D254" s="23"/>
       <c r="E254" s="23"/>
     </row>
-    <row r="255" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A255" s="23" t="s">
-        <v>340</v>
+    <row r="255" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A255" s="22" t="s">
+        <v>344</v>
       </c>
       <c r="B255" s="23" t="s">
-        <v>341</v>
+        <v>121</v>
       </c>
       <c r="C255" s="23"/>
       <c r="D255" s="23"/>
       <c r="E255" s="23"/>
     </row>
-    <row r="256" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A256" s="22" t="s">
-        <v>342</v>
+    <row r="256" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A256" s="23" t="s">
+        <v>345</v>
       </c>
       <c r="B256" s="23" t="s">
-        <v>343</v>
-      </c>
-      <c r="C256" s="23"/>
+        <v>125</v>
+      </c>
+      <c r="C256" s="23" t="s">
+        <v>126</v>
+      </c>
       <c r="D256" s="23"/>
       <c r="E256" s="23"/>
     </row>
-    <row r="257" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A257" s="22" t="s">
-        <v>344</v>
+    <row r="257" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A257" s="23" t="s">
+        <v>346</v>
       </c>
       <c r="B257" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="C257" s="23"/>
-      <c r="D257" s="23"/>
+        <v>347</v>
+      </c>
+      <c r="C257" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="D257" s="23" t="s">
+        <v>116</v>
+      </c>
       <c r="E257" s="23"/>
     </row>
-    <row r="258" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A258" s="23" t="s">
-        <v>345</v>
-      </c>
-      <c r="B258" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="C258" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="D258" s="23"/>
+        <v>346</v>
+      </c>
+      <c r="B258" s="23"/>
+      <c r="C258" s="23"/>
+      <c r="D258" s="23" t="s">
+        <v>117</v>
+      </c>
       <c r="E258" s="23"/>
     </row>
-    <row r="259" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A259" s="23" t="s">
-        <v>346</v>
-      </c>
-      <c r="B259" s="23" t="s">
-        <v>347</v>
-      </c>
-      <c r="C259" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="D259" s="23" t="s">
-        <v>116</v>
-      </c>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A259" s="22" t="s">
+        <v>348</v>
+      </c>
+      <c r="B259" s="23"/>
+      <c r="C259" s="23"/>
+      <c r="D259" s="22"/>
       <c r="E259" s="23"/>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A260" s="23" t="s">
-        <v>346</v>
-      </c>
-      <c r="B260" s="23"/>
+    <row r="260" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A260" s="22" t="s">
+        <v>349</v>
+      </c>
+      <c r="B260" s="23" t="s">
+        <v>161</v>
+      </c>
       <c r="C260" s="23"/>
-      <c r="D260" s="23" t="s">
-        <v>117</v>
-      </c>
+      <c r="D260" s="23"/>
       <c r="E260" s="23"/>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A261" s="22" t="s">
-        <v>348</v>
+      <c r="A261" s="23" t="s">
+        <v>350</v>
       </c>
       <c r="B261" s="23"/>
       <c r="C261" s="23"/>
-      <c r="D261" s="22"/>
+      <c r="D261" s="23"/>
       <c r="E261" s="23"/>
     </row>
-    <row r="262" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A262" s="22" t="s">
-        <v>349</v>
-      </c>
-      <c r="B262" s="23" t="s">
-        <v>161</v>
-      </c>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A262" s="23" t="s">
+        <v>351</v>
+      </c>
+      <c r="B262" s="23"/>
       <c r="C262" s="23"/>
       <c r="D262" s="23"/>
       <c r="E262" s="23"/>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A263" s="23" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B263" s="23"/>
       <c r="C263" s="23"/>
@@ -7521,8 +7513,8 @@
       <c r="E263" s="23"/>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A264" s="23" t="s">
-        <v>351</v>
+      <c r="A264" s="22" t="s">
+        <v>353</v>
       </c>
       <c r="B264" s="23"/>
       <c r="C264" s="23"/>
@@ -7530,8 +7522,8 @@
       <c r="E264" s="23"/>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A265" s="23" t="s">
-        <v>352</v>
+      <c r="A265" s="22" t="s">
+        <v>354</v>
       </c>
       <c r="B265" s="23"/>
       <c r="C265" s="23"/>
@@ -7540,7 +7532,7 @@
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A266" s="22" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B266" s="23"/>
       <c r="C266" s="23"/>
@@ -7549,7 +7541,7 @@
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A267" s="22" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B267" s="23"/>
       <c r="C267" s="23"/>
@@ -7558,7 +7550,7 @@
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A268" s="22" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B268" s="23"/>
       <c r="C268" s="23"/>
@@ -7567,45 +7559,45 @@
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A269" s="22" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B269" s="23"/>
       <c r="C269" s="23"/>
       <c r="D269" s="23"/>
       <c r="E269" s="23"/>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A270" s="22" t="s">
-        <v>357</v>
-      </c>
-      <c r="B270" s="23"/>
+    <row r="270" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A270" s="23" t="s">
+        <v>359</v>
+      </c>
+      <c r="B270" s="23" t="s">
+        <v>360</v>
+      </c>
       <c r="C270" s="23"/>
       <c r="D270" s="23"/>
       <c r="E270" s="23"/>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A271" s="22" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="B271" s="23"/>
       <c r="C271" s="23"/>
       <c r="D271" s="23"/>
       <c r="E271" s="23"/>
     </row>
-    <row r="272" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A272" s="23" t="s">
-        <v>359</v>
-      </c>
-      <c r="B272" s="23" t="s">
-        <v>360</v>
-      </c>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A272" s="22" t="s">
+        <v>362</v>
+      </c>
+      <c r="B272" s="23"/>
       <c r="C272" s="23"/>
       <c r="D272" s="23"/>
       <c r="E272" s="23"/>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A273" s="22" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B273" s="23"/>
       <c r="C273" s="23"/>
@@ -7614,7 +7606,7 @@
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A274" s="22" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="B274" s="23"/>
       <c r="C274" s="23"/>
@@ -7623,7 +7615,7 @@
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A275" s="22" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B275" s="23"/>
       <c r="C275" s="23"/>
@@ -7632,7 +7624,7 @@
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A276" s="22" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B276" s="23"/>
       <c r="C276" s="23"/>
@@ -7641,7 +7633,7 @@
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A277" s="22" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B277" s="23"/>
       <c r="C277" s="23"/>
@@ -7650,7 +7642,7 @@
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A278" s="22" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="B278" s="23"/>
       <c r="C278" s="23"/>
@@ -7659,7 +7651,7 @@
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A279" s="22" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B279" s="23"/>
       <c r="C279" s="23"/>
@@ -7667,8 +7659,8 @@
       <c r="E279" s="23"/>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A280" s="22" t="s">
-        <v>368</v>
+      <c r="A280" s="23" t="s">
+        <v>370</v>
       </c>
       <c r="B280" s="23"/>
       <c r="C280" s="23"/>
@@ -7676,8 +7668,8 @@
       <c r="E280" s="23"/>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A281" s="22" t="s">
-        <v>369</v>
+      <c r="A281" s="23" t="s">
+        <v>371</v>
       </c>
       <c r="B281" s="23"/>
       <c r="C281" s="23"/>
@@ -7686,70 +7678,74 @@
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A282" s="23" t="s">
-        <v>370</v>
+        <v>1307</v>
       </c>
       <c r="B282" s="23"/>
       <c r="C282" s="23"/>
       <c r="D282" s="23"/>
       <c r="E282" s="23"/>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A283" s="23" t="s">
-        <v>371</v>
-      </c>
-      <c r="B283" s="23"/>
+        <v>373</v>
+      </c>
+      <c r="B283" s="23" t="s">
+        <v>251</v>
+      </c>
       <c r="C283" s="23"/>
       <c r="D283" s="23"/>
       <c r="E283" s="23"/>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A284" s="23" t="s">
-        <v>1307</v>
-      </c>
-      <c r="B284" s="23"/>
+        <v>374</v>
+      </c>
+      <c r="B284" s="23" t="s">
+        <v>253</v>
+      </c>
       <c r="C284" s="23"/>
       <c r="D284" s="23"/>
       <c r="E284" s="23"/>
     </row>
-    <row r="285" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A285" s="23" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B285" s="23" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="C285" s="23"/>
       <c r="D285" s="23"/>
       <c r="E285" s="23"/>
     </row>
-    <row r="286" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A286" s="23" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B286" s="23" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C286" s="23"/>
       <c r="D286" s="23"/>
       <c r="E286" s="23"/>
     </row>
-    <row r="287" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A287" s="23" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B287" s="23" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="C287" s="23"/>
       <c r="D287" s="23"/>
       <c r="E287" s="23"/>
     </row>
-    <row r="288" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A288" s="23" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B288" s="23" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="C288" s="23"/>
       <c r="D288" s="23"/>
@@ -7757,21 +7753,21 @@
     </row>
     <row r="289" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A289" s="23" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B289" s="23" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="C289" s="23"/>
       <c r="D289" s="23"/>
       <c r="E289" s="23"/>
     </row>
-    <row r="290" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A290" s="23" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B290" s="23" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="C290" s="23"/>
       <c r="D290" s="23"/>
@@ -7779,67 +7775,67 @@
     </row>
     <row r="291" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A291" s="23" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B291" s="23" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="C291" s="23"/>
       <c r="D291" s="23"/>
       <c r="E291" s="23"/>
     </row>
-    <row r="292" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A292" s="23" t="s">
-        <v>380</v>
-      </c>
-      <c r="B292" s="23" t="s">
-        <v>265</v>
-      </c>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A292" s="22" t="s">
+        <v>382</v>
+      </c>
+      <c r="B292" s="23"/>
       <c r="C292" s="23"/>
       <c r="D292" s="23"/>
       <c r="E292" s="23"/>
     </row>
-    <row r="293" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A293" s="23" t="s">
-        <v>381</v>
-      </c>
-      <c r="B293" s="23" t="s">
-        <v>267</v>
-      </c>
+    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A293" s="22" t="s">
+        <v>383</v>
+      </c>
+      <c r="B293" s="23"/>
       <c r="C293" s="23"/>
       <c r="D293" s="23"/>
       <c r="E293" s="23"/>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A294" s="22" t="s">
-        <v>382</v>
-      </c>
-      <c r="B294" s="23"/>
-      <c r="C294" s="23"/>
-      <c r="D294" s="23"/>
+    <row r="294" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A294" s="23" t="s">
+        <v>384</v>
+      </c>
+      <c r="B294" s="23" t="s">
+        <v>385</v>
+      </c>
+      <c r="C294" s="23" t="s">
+        <v>386</v>
+      </c>
+      <c r="D294" s="23" t="s">
+        <v>387</v>
+      </c>
       <c r="E294" s="23"/>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A295" s="22" t="s">
-        <v>383</v>
+      <c r="A295" s="23" t="s">
+        <v>384</v>
       </c>
       <c r="B295" s="23"/>
       <c r="C295" s="23"/>
-      <c r="D295" s="23"/>
+      <c r="D295" s="23" t="s">
+        <v>388</v>
+      </c>
       <c r="E295" s="23"/>
     </row>
-    <row r="296" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A296" s="23" t="s">
         <v>384</v>
       </c>
-      <c r="B296" s="23" t="s">
-        <v>385</v>
-      </c>
-      <c r="C296" s="23" t="s">
-        <v>386</v>
-      </c>
+      <c r="B296" s="23"/>
+      <c r="C296" s="23"/>
       <c r="D296" s="23" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="E296" s="23"/>
     </row>
@@ -7850,7 +7846,7 @@
       <c r="B297" s="23"/>
       <c r="C297" s="23"/>
       <c r="D297" s="23" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="E297" s="23"/>
     </row>
@@ -7861,50 +7857,52 @@
       <c r="B298" s="23"/>
       <c r="C298" s="23"/>
       <c r="D298" s="23" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="E298" s="23"/>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A299" s="23" t="s">
-        <v>384</v>
-      </c>
-      <c r="B299" s="23"/>
+        <v>392</v>
+      </c>
+      <c r="B299" s="23" t="s">
+        <v>308</v>
+      </c>
       <c r="C299" s="23"/>
       <c r="D299" s="23" t="s">
-        <v>390</v>
-      </c>
-      <c r="E299" s="23"/>
+        <v>207</v>
+      </c>
+      <c r="E299" s="23" t="s">
+        <v>393</v>
+      </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A300" s="23" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
       <c r="B300" s="23"/>
       <c r="C300" s="23"/>
       <c r="D300" s="23" t="s">
-        <v>391</v>
+        <v>209</v>
       </c>
       <c r="E300" s="23"/>
     </row>
-    <row r="301" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A301" s="23" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="B301" s="23" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="C301" s="23"/>
       <c r="D301" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="E301" s="23" t="s">
-        <v>393</v>
-      </c>
+      <c r="E301" s="23"/>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A302" s="23" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="B302" s="23"/>
       <c r="C302" s="23"/>
@@ -7913,12 +7911,12 @@
       </c>
       <c r="E302" s="23"/>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A303" s="23" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B303" s="23" t="s">
-        <v>311</v>
+        <v>213</v>
       </c>
       <c r="C303" s="23"/>
       <c r="D303" s="23" t="s">
@@ -7928,7 +7926,7 @@
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A304" s="23" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B304" s="23"/>
       <c r="C304" s="23"/>
@@ -7937,12 +7935,12 @@
       </c>
       <c r="E304" s="23"/>
     </row>
-    <row r="305" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A305" s="23" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B305" s="23" t="s">
-        <v>213</v>
+        <v>44</v>
       </c>
       <c r="C305" s="23"/>
       <c r="D305" s="23" t="s">
@@ -7952,7 +7950,7 @@
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A306" s="23" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B306" s="23"/>
       <c r="C306" s="23"/>
@@ -7963,93 +7961,91 @@
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A307" s="23" t="s">
-        <v>396</v>
+        <v>420</v>
       </c>
       <c r="B307" s="23" t="s">
-        <v>44</v>
+        <v>421</v>
       </c>
       <c r="C307" s="23"/>
-      <c r="D307" s="23" t="s">
-        <v>207</v>
-      </c>
+      <c r="D307" s="23"/>
       <c r="E307" s="23"/>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A308" s="23" t="s">
-        <v>396</v>
-      </c>
-      <c r="B308" s="23"/>
-      <c r="C308" s="23"/>
+        <v>397</v>
+      </c>
+      <c r="B308" s="23" t="s">
+        <v>398</v>
+      </c>
+      <c r="C308" s="23" t="s">
+        <v>399</v>
+      </c>
       <c r="D308" s="23" t="s">
-        <v>209</v>
+        <v>400</v>
       </c>
       <c r="E308" s="23"/>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A309" s="23" t="s">
-        <v>420</v>
-      </c>
-      <c r="B309" s="23" t="s">
-        <v>421</v>
-      </c>
+        <v>397</v>
+      </c>
+      <c r="B309" s="23"/>
       <c r="C309" s="23"/>
-      <c r="D309" s="23"/>
+      <c r="D309" s="23" t="s">
+        <v>401</v>
+      </c>
       <c r="E309" s="23"/>
     </row>
     <row r="310" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A310" s="23" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
       <c r="B310" s="23" t="s">
-        <v>398</v>
-      </c>
-      <c r="C310" s="23" t="s">
-        <v>399</v>
-      </c>
-      <c r="D310" s="23" t="s">
-        <v>400</v>
-      </c>
+        <v>403</v>
+      </c>
+      <c r="C310" s="23"/>
+      <c r="D310" s="23"/>
       <c r="E310" s="23"/>
     </row>
     <row r="311" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A311" s="23" t="s">
-        <v>397</v>
-      </c>
-      <c r="B311" s="23"/>
+        <v>404</v>
+      </c>
+      <c r="B311" s="23" t="s">
+        <v>405</v>
+      </c>
       <c r="C311" s="23"/>
-      <c r="D311" s="23" t="s">
-        <v>401</v>
-      </c>
+      <c r="D311" s="23"/>
       <c r="E311" s="23"/>
     </row>
     <row r="312" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A312" s="23" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="B312" s="23" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="C312" s="23"/>
       <c r="D312" s="23"/>
       <c r="E312" s="23"/>
     </row>
-    <row r="313" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A313" s="23" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="B313" s="23" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="C313" s="23"/>
       <c r="D313" s="23"/>
       <c r="E313" s="23"/>
     </row>
-    <row r="314" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A314" s="23" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="B314" s="23" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="C314" s="23"/>
       <c r="D314" s="23"/>
@@ -8057,10 +8053,10 @@
     </row>
     <row r="315" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A315" s="23" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="B315" s="23" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="C315" s="23"/>
       <c r="D315" s="23"/>
@@ -8068,10 +8064,10 @@
     </row>
     <row r="316" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A316" s="23" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="B316" s="23" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="C316" s="23"/>
       <c r="D316" s="23"/>
@@ -8079,52 +8075,30 @@
     </row>
     <row r="317" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A317" s="23" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="B317" s="23" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="C317" s="23"/>
       <c r="D317" s="23"/>
       <c r="E317" s="23"/>
     </row>
-    <row r="318" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A318" s="23" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="B318" s="23" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="C318" s="23"/>
       <c r="D318" s="23"/>
       <c r="E318" s="23"/>
     </row>
-    <row r="319" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A319" s="23" t="s">
-        <v>416</v>
-      </c>
-      <c r="B319" s="23" t="s">
-        <v>417</v>
-      </c>
+    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C319" s="23"/>
       <c r="D319" s="23"/>
       <c r="E319" s="23"/>
-    </row>
-    <row r="320" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A320" s="23" t="s">
-        <v>418</v>
-      </c>
-      <c r="B320" s="23" t="s">
-        <v>419</v>
-      </c>
-      <c r="C320" s="23"/>
-      <c r="D320" s="23"/>
-      <c r="E320" s="23"/>
-    </row>
-    <row r="321" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C321" s="23"/>
-      <c r="D321" s="23"/>
-      <c r="E321" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>